<commit_message>
Añadir Base para Calendario
</commit_message>
<xml_diff>
--- a/Calendario.xlsx
+++ b/Calendario.xlsx
@@ -19,16 +19,96 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+  <si>
+    <t xml:space="preserve">Horas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6 am - 7 am</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7 am – 8 am</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8 am – 9 am</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9 am – 10 am</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10 am – 11 am</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11 am – 12 am</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12 am – 1 pm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 pm – 2 pm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 pm – 3 pm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 pm – 4 pm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4 pm – 5 pm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5 pm – 6 pm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6 pm – 7 pm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7 pm – 8 pm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8 pm – 9 pm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9 pm - 10 pm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lunes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Martes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Miercoles</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jueves</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Viernes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sabado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Domingo</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="mm/dd/yy"/>
+    <numFmt numFmtId="166" formatCode="hh:mm:ss\ AM/PM"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -44,6 +124,21 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <i val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -54,7 +149,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -62,6 +157,13 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right style="hair"/>
+      <top style="hair"/>
+      <bottom style="hair"/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -88,8 +190,28 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -110,14 +232,223 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="B2:R9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <sheetData/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="6.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="11.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="0" width="12.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="13.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="12.68"/>
+  </cols>
+  <sheetData>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="O2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="R2" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="4"/>
+      <c r="M3" s="4"/>
+      <c r="N3" s="4"/>
+      <c r="O3" s="4"/>
+      <c r="P3" s="4"/>
+      <c r="Q3" s="4"/>
+      <c r="R3" s="4"/>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="4"/>
+      <c r="M4" s="4"/>
+      <c r="N4" s="4"/>
+      <c r="O4" s="4"/>
+      <c r="P4" s="4"/>
+      <c r="Q4" s="4"/>
+      <c r="R4" s="4"/>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
+      <c r="L5" s="4"/>
+      <c r="M5" s="4"/>
+      <c r="N5" s="4"/>
+      <c r="O5" s="4"/>
+      <c r="P5" s="4"/>
+      <c r="Q5" s="4"/>
+      <c r="R5" s="4"/>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
+      <c r="L6" s="4"/>
+      <c r="M6" s="4"/>
+      <c r="N6" s="4"/>
+      <c r="O6" s="4"/>
+      <c r="P6" s="4"/>
+      <c r="Q6" s="4"/>
+      <c r="R6" s="4"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="4"/>
+      <c r="M7" s="4"/>
+      <c r="N7" s="4"/>
+      <c r="O7" s="4"/>
+      <c r="P7" s="4"/>
+      <c r="Q7" s="4"/>
+      <c r="R7" s="4"/>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4"/>
+      <c r="L8" s="4"/>
+      <c r="M8" s="4"/>
+      <c r="N8" s="4"/>
+      <c r="O8" s="4"/>
+      <c r="P8" s="4"/>
+      <c r="Q8" s="4"/>
+      <c r="R8" s="4"/>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B9" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="4"/>
+      <c r="K9" s="4"/>
+      <c r="L9" s="4"/>
+      <c r="M9" s="4"/>
+      <c r="N9" s="4"/>
+      <c r="O9" s="4"/>
+      <c r="P9" s="4"/>
+      <c r="Q9" s="4"/>
+      <c r="R9" s="4"/>
+    </row>
+  </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
Add: Estudio Lunes, Clases se ven virtuales Martes
</commit_message>
<xml_diff>
--- a/Calendario.xlsx
+++ b/Calendario.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="70">
   <si>
     <t xml:space="preserve">             Dias</t>
   </si>
@@ -79,6 +79,9 @@
     <t xml:space="preserve">7 a.m</t>
   </si>
   <si>
+    <t xml:space="preserve">Despertarme</t>
+  </si>
+  <si>
     <t xml:space="preserve">Ir a la Universidad</t>
   </si>
   <si>
@@ -106,12 +109,15 @@
     <t xml:space="preserve">12 p.m</t>
   </si>
   <si>
+    <t xml:space="preserve">Hacer Tarea Laboratorio Informática 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clase Cálculo 1</t>
+  </si>
+  <si>
     <t xml:space="preserve">Devolverme de la Universidad</t>
   </si>
   <si>
-    <t xml:space="preserve">Clase Cálculo 1</t>
-  </si>
-  <si>
     <t xml:space="preserve">1 p.m</t>
   </si>
   <si>
@@ -133,6 +139,9 @@
     <t xml:space="preserve">6 p.m</t>
   </si>
   <si>
+    <t xml:space="preserve">Hacer tarea Laboratorio Informática 2</t>
+  </si>
+  <si>
     <t xml:space="preserve">Laboratorio Informática 2</t>
   </si>
   <si>
@@ -169,6 +178,12 @@
     <t xml:space="preserve">26 Febrero</t>
   </si>
   <si>
+    <t xml:space="preserve">Clase Álgebra 1 y Quizz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quizz Cálculo 1</t>
+  </si>
+  <si>
     <t xml:space="preserve">27 Febrero</t>
   </si>
   <si>
@@ -190,6 +205,9 @@
     <t xml:space="preserve">5 Marzo</t>
   </si>
   <si>
+    <t xml:space="preserve">Parcial Álgebra 1</t>
+  </si>
+  <si>
     <t xml:space="preserve">6 Marzo</t>
   </si>
   <si>
@@ -209,6 +227,9 @@
   </si>
   <si>
     <t xml:space="preserve">12 Marzo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Parcial Cálculo 1</t>
   </si>
 </sst>
 </file>
@@ -490,17 +511,15 @@
   <dimension ref="B2:J80"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K10" activeCellId="0" sqref="K10"/>
+      <selection pane="topLeft" activeCell="J10" activeCellId="0" sqref="J10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="6.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="25.6"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="24.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="25.6"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="24.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="31.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="31.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="5" style="0" width="25.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="13.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="12.68"/>
   </cols>
@@ -564,9 +583,7 @@
         <v>16</v>
       </c>
       <c r="C4" s="10"/>
-      <c r="D4" s="10" t="s">
-        <v>17</v>
-      </c>
+      <c r="D4" s="10"/>
       <c r="E4" s="10"/>
       <c r="F4" s="10" t="s">
         <v>17</v>
@@ -586,7 +603,7 @@
       </c>
       <c r="E5" s="10"/>
       <c r="F5" s="10" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G5" s="10"/>
       <c r="H5" s="10"/>
@@ -595,17 +612,17 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C6" s="10"/>
       <c r="D6" s="12" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E6" s="10" t="s">
         <v>17</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G6" s="10" t="s">
         <v>17</v>
@@ -616,16 +633,16 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="9" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C7" s="10"/>
       <c r="D7" s="12"/>
       <c r="E7" s="10" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F7" s="12"/>
       <c r="G7" s="10" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H7" s="10"/>
       <c r="I7" s="10"/>
@@ -633,20 +650,20 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="11" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C8" s="10"/>
       <c r="D8" s="12" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E8" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="F8" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="F8" s="12" t="s">
-        <v>24</v>
-      </c>
       <c r="G8" s="12" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H8" s="10"/>
       <c r="I8" s="10"/>
@@ -654,7 +671,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="11" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C9" s="10"/>
       <c r="D9" s="12"/>
@@ -667,30 +684,30 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="9" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C10" s="13"/>
-      <c r="D10" s="13" t="s">
-        <v>28</v>
+      <c r="D10" s="12" t="s">
+        <v>29</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F10" s="13" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="G10" s="12" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H10" s="13"/>
       <c r="I10" s="13"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="11" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C11" s="13"/>
-      <c r="D11" s="13"/>
+      <c r="D11" s="12"/>
       <c r="E11" s="12"/>
       <c r="F11" s="13"/>
       <c r="G11" s="12"/>
@@ -699,12 +716,12 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" s="13"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="13" t="s">
         <v>31</v>
-      </c>
-      <c r="C12" s="13"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13" t="s">
-        <v>28</v>
       </c>
       <c r="F12" s="13"/>
       <c r="G12" s="13"/>
@@ -713,10 +730,10 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="11" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C13" s="13"/>
-      <c r="D13" s="13"/>
+      <c r="D13" s="12"/>
       <c r="E13" s="13"/>
       <c r="F13" s="13"/>
       <c r="G13" s="13"/>
@@ -725,7 +742,7 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="11" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C14" s="13"/>
       <c r="D14" s="13"/>
@@ -737,13 +754,13 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="11" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C15" s="13"/>
       <c r="D15" s="13"/>
       <c r="E15" s="13"/>
       <c r="F15" s="12" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="G15" s="13"/>
       <c r="H15" s="13"/>
@@ -751,23 +768,25 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="C16" s="13"/>
+        <v>38</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>39</v>
+      </c>
       <c r="D16" s="13"/>
       <c r="E16" s="13"/>
       <c r="F16" s="12"/>
       <c r="G16" s="12" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="H16" s="13"/>
       <c r="I16" s="13"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="C17" s="13"/>
+        <v>41</v>
+      </c>
+      <c r="C17" s="12"/>
       <c r="D17" s="13"/>
       <c r="E17" s="13"/>
       <c r="F17" s="13"/>
@@ -777,9 +796,9 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="C18" s="13"/>
+        <v>42</v>
+      </c>
+      <c r="C18" s="12"/>
       <c r="D18" s="13"/>
       <c r="E18" s="13"/>
       <c r="F18" s="13"/>
@@ -789,21 +808,21 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="C19" s="13"/>
+        <v>43</v>
+      </c>
+      <c r="C19" s="12"/>
       <c r="D19" s="13"/>
       <c r="E19" s="13"/>
       <c r="F19" s="13"/>
       <c r="G19" s="13" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="H19" s="13"/>
       <c r="I19" s="13"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="11" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="C20" s="13"/>
       <c r="D20" s="13"/>
@@ -844,25 +863,25 @@
         <v>8</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="G23" s="6" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="H23" s="7" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="I23" s="6" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -887,11 +906,11 @@
       </c>
       <c r="C25" s="10"/>
       <c r="D25" s="10" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E25" s="10"/>
       <c r="F25" s="10" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G25" s="10"/>
       <c r="H25" s="10"/>
@@ -899,17 +918,17 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C26" s="10"/>
       <c r="D26" s="12" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E26" s="10" t="s">
         <v>17</v>
       </c>
       <c r="F26" s="12" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G26" s="10" t="s">
         <v>17</v>
@@ -919,43 +938,43 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="9" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C27" s="10"/>
       <c r="D27" s="12"/>
       <c r="E27" s="10" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F27" s="12"/>
       <c r="G27" s="10" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H27" s="10"/>
       <c r="I27" s="10"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="11" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C28" s="10"/>
       <c r="D28" s="12" t="s">
-        <v>24</v>
+        <v>52</v>
       </c>
       <c r="E28" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="F28" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="F28" s="12" t="s">
-        <v>24</v>
-      </c>
       <c r="G28" s="12" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H28" s="10"/>
       <c r="I28" s="10"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="11" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C29" s="10"/>
       <c r="D29" s="12"/>
@@ -967,27 +986,27 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="9" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C30" s="13"/>
       <c r="D30" s="13" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="E30" s="12" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F30" s="13" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="G30" s="12" t="s">
-        <v>29</v>
+        <v>53</v>
       </c>
       <c r="H30" s="13"/>
       <c r="I30" s="13"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="11" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C31" s="13"/>
       <c r="D31" s="13"/>
@@ -999,12 +1018,12 @@
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="11" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C32" s="13"/>
       <c r="D32" s="13"/>
       <c r="E32" s="13" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="F32" s="13"/>
       <c r="G32" s="13"/>
@@ -1013,7 +1032,7 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="11" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C33" s="13"/>
       <c r="D33" s="13"/>
@@ -1025,7 +1044,7 @@
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="11" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C34" s="13"/>
       <c r="D34" s="13"/>
@@ -1037,13 +1056,13 @@
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="11" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C35" s="13"/>
       <c r="D35" s="13"/>
       <c r="E35" s="13"/>
       <c r="F35" s="12" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="G35" s="13"/>
       <c r="H35" s="13"/>
@@ -1051,21 +1070,21 @@
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="11" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C36" s="13"/>
       <c r="D36" s="13"/>
       <c r="E36" s="13"/>
       <c r="F36" s="12"/>
       <c r="G36" s="12" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="H36" s="13"/>
       <c r="I36" s="13"/>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="11" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C37" s="13"/>
       <c r="D37" s="13"/>
@@ -1077,7 +1096,7 @@
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B38" s="11" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="C38" s="13"/>
       <c r="D38" s="13"/>
@@ -1089,21 +1108,21 @@
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B39" s="11" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C39" s="13"/>
       <c r="D39" s="13"/>
       <c r="E39" s="13"/>
       <c r="F39" s="13"/>
       <c r="G39" s="13" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="H39" s="13"/>
       <c r="I39" s="13"/>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B40" s="11" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="C40" s="13"/>
       <c r="D40" s="13"/>
@@ -1145,25 +1164,25 @@
         <v>8</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="D43" s="7" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="E43" s="6" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="F43" s="6" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="G43" s="6" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="H43" s="6" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="I43" s="6" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="J43" s="8"/>
     </row>
@@ -1190,11 +1209,11 @@
       </c>
       <c r="C45" s="10"/>
       <c r="D45" s="10" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E45" s="10"/>
       <c r="F45" s="10" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G45" s="10"/>
       <c r="H45" s="10"/>
@@ -1203,17 +1222,17 @@
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B46" s="11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C46" s="10"/>
       <c r="D46" s="12" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E46" s="10" t="s">
         <v>17</v>
       </c>
       <c r="F46" s="12" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G46" s="10" t="s">
         <v>17</v>
@@ -1224,16 +1243,16 @@
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B47" s="9" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C47" s="10"/>
       <c r="D47" s="12"/>
       <c r="E47" s="10" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F47" s="12"/>
       <c r="G47" s="10" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H47" s="10"/>
       <c r="I47" s="10"/>
@@ -1241,20 +1260,20 @@
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B48" s="11" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C48" s="10"/>
       <c r="D48" s="12" t="s">
-        <v>24</v>
+        <v>61</v>
       </c>
       <c r="E48" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="F48" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="F48" s="12" t="s">
-        <v>24</v>
-      </c>
       <c r="G48" s="12" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H48" s="10"/>
       <c r="I48" s="10"/>
@@ -1262,7 +1281,7 @@
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B49" s="11" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C49" s="10"/>
       <c r="D49" s="12"/>
@@ -1275,27 +1294,27 @@
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B50" s="9" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C50" s="13"/>
       <c r="D50" s="13" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="E50" s="12" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F50" s="13" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="G50" s="12" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H50" s="13"/>
       <c r="I50" s="13"/>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B51" s="11" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C51" s="13"/>
       <c r="D51" s="13"/>
@@ -1307,12 +1326,12 @@
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B52" s="11" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C52" s="13"/>
       <c r="D52" s="13"/>
       <c r="E52" s="13" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="F52" s="13"/>
       <c r="G52" s="13"/>
@@ -1321,7 +1340,7 @@
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B53" s="11" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C53" s="13"/>
       <c r="D53" s="13"/>
@@ -1333,7 +1352,7 @@
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B54" s="11" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C54" s="13"/>
       <c r="D54" s="13"/>
@@ -1345,13 +1364,13 @@
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B55" s="11" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C55" s="13"/>
       <c r="D55" s="13"/>
       <c r="E55" s="13"/>
       <c r="F55" s="12" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="G55" s="13"/>
       <c r="H55" s="13"/>
@@ -1359,21 +1378,21 @@
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B56" s="11" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C56" s="13"/>
       <c r="D56" s="13"/>
       <c r="E56" s="13"/>
       <c r="F56" s="12"/>
       <c r="G56" s="12" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="H56" s="13"/>
       <c r="I56" s="13"/>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B57" s="11" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C57" s="13"/>
       <c r="D57" s="13"/>
@@ -1385,7 +1404,7 @@
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B58" s="11" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="C58" s="13"/>
       <c r="D58" s="13"/>
@@ -1397,21 +1416,21 @@
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B59" s="11" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C59" s="13"/>
       <c r="D59" s="13"/>
       <c r="E59" s="13"/>
       <c r="F59" s="13"/>
       <c r="G59" s="13" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="H59" s="13"/>
       <c r="I59" s="13"/>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B60" s="11" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="C60" s="13"/>
       <c r="D60" s="13"/>
@@ -1452,25 +1471,25 @@
         <v>8</v>
       </c>
       <c r="C63" s="6" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="D63" s="7" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="E63" s="6" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="F63" s="7" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="G63" s="6" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="H63" s="7" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="I63" s="6" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1495,11 +1514,11 @@
       </c>
       <c r="C65" s="10"/>
       <c r="D65" s="10" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E65" s="10"/>
       <c r="F65" s="10" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G65" s="10"/>
       <c r="H65" s="10"/>
@@ -1507,17 +1526,17 @@
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B66" s="11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C66" s="10"/>
       <c r="D66" s="12" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E66" s="10" t="s">
         <v>17</v>
       </c>
       <c r="F66" s="12" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G66" s="10" t="s">
         <v>17</v>
@@ -1527,43 +1546,43 @@
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B67" s="9" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C67" s="10"/>
       <c r="D67" s="12"/>
       <c r="E67" s="10" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F67" s="12"/>
       <c r="G67" s="10" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H67" s="10"/>
       <c r="I67" s="10"/>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B68" s="11" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C68" s="10"/>
       <c r="D68" s="12" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E68" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="F68" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="F68" s="12" t="s">
-        <v>24</v>
-      </c>
       <c r="G68" s="12" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H68" s="10"/>
       <c r="I68" s="10"/>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B69" s="11" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C69" s="10"/>
       <c r="D69" s="12"/>
@@ -1575,27 +1594,27 @@
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B70" s="9" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C70" s="13"/>
       <c r="D70" s="13" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="E70" s="12" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F70" s="13" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="G70" s="12" t="s">
-        <v>29</v>
+        <v>69</v>
       </c>
       <c r="H70" s="13"/>
       <c r="I70" s="13"/>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B71" s="11" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C71" s="13"/>
       <c r="D71" s="13"/>
@@ -1607,12 +1626,12 @@
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B72" s="11" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C72" s="13"/>
       <c r="D72" s="13"/>
       <c r="E72" s="13" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="F72" s="13"/>
       <c r="G72" s="13"/>
@@ -1621,7 +1640,7 @@
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B73" s="11" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C73" s="13"/>
       <c r="D73" s="13"/>
@@ -1633,7 +1652,7 @@
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B74" s="11" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C74" s="13"/>
       <c r="D74" s="13"/>
@@ -1645,13 +1664,13 @@
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B75" s="11" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C75" s="13"/>
       <c r="D75" s="13"/>
       <c r="E75" s="13"/>
       <c r="F75" s="12" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="G75" s="13"/>
       <c r="H75" s="13"/>
@@ -1659,21 +1678,21 @@
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B76" s="11" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C76" s="13"/>
       <c r="D76" s="13"/>
       <c r="E76" s="13"/>
       <c r="F76" s="12"/>
       <c r="G76" s="12" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="H76" s="13"/>
       <c r="I76" s="13"/>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B77" s="11" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C77" s="13"/>
       <c r="D77" s="13"/>
@@ -1685,7 +1704,7 @@
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B78" s="11" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="C78" s="13"/>
       <c r="D78" s="13"/>
@@ -1697,21 +1716,21 @@
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B79" s="11" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C79" s="13"/>
       <c r="D79" s="13"/>
       <c r="E79" s="13"/>
       <c r="F79" s="13"/>
       <c r="G79" s="13" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="H79" s="13"/>
       <c r="I79" s="13"/>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B80" s="11" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="C80" s="13"/>
       <c r="D80" s="13"/>
@@ -1722,16 +1741,18 @@
       <c r="I80" s="13"/>
     </row>
   </sheetData>
-  <mergeCells count="40">
+  <mergeCells count="42">
     <mergeCell ref="D6:D7"/>
     <mergeCell ref="F6:F7"/>
     <mergeCell ref="D8:D9"/>
     <mergeCell ref="E8:E9"/>
     <mergeCell ref="F8:F9"/>
     <mergeCell ref="G8:G9"/>
+    <mergeCell ref="D10:D13"/>
     <mergeCell ref="E10:E11"/>
     <mergeCell ref="G10:G11"/>
     <mergeCell ref="F15:F16"/>
+    <mergeCell ref="C16:C19"/>
     <mergeCell ref="G16:G18"/>
     <mergeCell ref="D26:D27"/>
     <mergeCell ref="F26:F27"/>

</xml_diff>

<commit_message>
Cambio: Por si no voy 15_Feb por manifestaciones que pueden hacer en la universidad
</commit_message>
<xml_diff>
--- a/Calendario.xlsx
+++ b/Calendario.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="71">
   <si>
     <t xml:space="preserve">             Dias</t>
   </si>
@@ -112,10 +112,13 @@
     <t xml:space="preserve">Hacer Tarea Laboratorio Informática 2</t>
   </si>
   <si>
+    <t xml:space="preserve">Estudiar Cálculo 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Devolverme de la Universidad</t>
+  </si>
+  <si>
     <t xml:space="preserve">Clase Cálculo 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Devolverme de la Universidad</t>
   </si>
   <si>
     <t xml:space="preserve">1 p.m</t>
@@ -511,10 +514,10 @@
   <dimension ref="B2:J80"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J10" activeCellId="0" sqref="J10"/>
+      <selection pane="topLeft" activeCell="J11" activeCellId="0" sqref="J11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="31.43"/>
@@ -618,9 +621,7 @@
       <c r="D6" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="E6" s="10" t="s">
-        <v>17</v>
-      </c>
+      <c r="E6" s="10"/>
       <c r="F6" s="12" t="s">
         <v>22</v>
       </c>
@@ -638,7 +639,7 @@
       <c r="C7" s="10"/>
       <c r="D7" s="12"/>
       <c r="E7" s="10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F7" s="12"/>
       <c r="G7" s="10" t="s">
@@ -697,14 +698,14 @@
         <v>31</v>
       </c>
       <c r="G10" s="12" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H10" s="13"/>
       <c r="I10" s="13"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="11" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C11" s="13"/>
       <c r="D11" s="12"/>
@@ -716,13 +717,11 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="11" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C12" s="13"/>
       <c r="D12" s="12"/>
-      <c r="E12" s="13" t="s">
-        <v>31</v>
-      </c>
+      <c r="E12" s="13"/>
       <c r="F12" s="13"/>
       <c r="G12" s="13"/>
       <c r="H12" s="13"/>
@@ -730,7 +729,7 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="11" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C13" s="13"/>
       <c r="D13" s="12"/>
@@ -742,7 +741,7 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="11" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C14" s="13"/>
       <c r="D14" s="13"/>
@@ -754,13 +753,13 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="11" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C15" s="13"/>
       <c r="D15" s="13"/>
       <c r="E15" s="13"/>
       <c r="F15" s="12" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G15" s="13"/>
       <c r="H15" s="13"/>
@@ -768,23 +767,23 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="11" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D16" s="13"/>
       <c r="E16" s="13"/>
       <c r="F16" s="12"/>
       <c r="G16" s="12" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="H16" s="13"/>
       <c r="I16" s="13"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="11" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C17" s="12"/>
       <c r="D17" s="13"/>
@@ -796,7 +795,7 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="11" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C18" s="12"/>
       <c r="D18" s="13"/>
@@ -808,7 +807,7 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="11" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C19" s="12"/>
       <c r="D19" s="13"/>
@@ -822,7 +821,7 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="11" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C20" s="13"/>
       <c r="D20" s="13"/>
@@ -863,25 +862,25 @@
         <v>8</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="G23" s="6" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="H23" s="7" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="I23" s="6" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -958,7 +957,7 @@
       </c>
       <c r="C28" s="10"/>
       <c r="D28" s="12" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E28" s="12" t="s">
         <v>26</v>
@@ -993,20 +992,20 @@
         <v>31</v>
       </c>
       <c r="E30" s="12" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F30" s="13" t="s">
         <v>31</v>
       </c>
       <c r="G30" s="12" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="H30" s="13"/>
       <c r="I30" s="13"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="11" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C31" s="13"/>
       <c r="D31" s="13"/>
@@ -1018,7 +1017,7 @@
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="11" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C32" s="13"/>
       <c r="D32" s="13"/>
@@ -1032,7 +1031,7 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="11" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C33" s="13"/>
       <c r="D33" s="13"/>
@@ -1044,7 +1043,7 @@
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="11" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C34" s="13"/>
       <c r="D34" s="13"/>
@@ -1056,13 +1055,13 @@
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="11" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C35" s="13"/>
       <c r="D35" s="13"/>
       <c r="E35" s="13"/>
       <c r="F35" s="12" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G35" s="13"/>
       <c r="H35" s="13"/>
@@ -1070,21 +1069,21 @@
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="11" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C36" s="13"/>
       <c r="D36" s="13"/>
       <c r="E36" s="13"/>
       <c r="F36" s="12"/>
       <c r="G36" s="12" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="H36" s="13"/>
       <c r="I36" s="13"/>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="11" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C37" s="13"/>
       <c r="D37" s="13"/>
@@ -1096,7 +1095,7 @@
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B38" s="11" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C38" s="13"/>
       <c r="D38" s="13"/>
@@ -1108,7 +1107,7 @@
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B39" s="11" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C39" s="13"/>
       <c r="D39" s="13"/>
@@ -1122,7 +1121,7 @@
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B40" s="11" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C40" s="13"/>
       <c r="D40" s="13"/>
@@ -1164,25 +1163,25 @@
         <v>8</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D43" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E43" s="6" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F43" s="6" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="G43" s="6" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="H43" s="6" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="I43" s="6" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="J43" s="8"/>
     </row>
@@ -1264,7 +1263,7 @@
       </c>
       <c r="C48" s="10"/>
       <c r="D48" s="12" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E48" s="12" t="s">
         <v>26</v>
@@ -1301,20 +1300,20 @@
         <v>31</v>
       </c>
       <c r="E50" s="12" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F50" s="13" t="s">
         <v>31</v>
       </c>
       <c r="G50" s="12" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H50" s="13"/>
       <c r="I50" s="13"/>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B51" s="11" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C51" s="13"/>
       <c r="D51" s="13"/>
@@ -1326,7 +1325,7 @@
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B52" s="11" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C52" s="13"/>
       <c r="D52" s="13"/>
@@ -1340,7 +1339,7 @@
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B53" s="11" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C53" s="13"/>
       <c r="D53" s="13"/>
@@ -1352,7 +1351,7 @@
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B54" s="11" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C54" s="13"/>
       <c r="D54" s="13"/>
@@ -1364,13 +1363,13 @@
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B55" s="11" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C55" s="13"/>
       <c r="D55" s="13"/>
       <c r="E55" s="13"/>
       <c r="F55" s="12" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G55" s="13"/>
       <c r="H55" s="13"/>
@@ -1378,21 +1377,21 @@
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B56" s="11" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C56" s="13"/>
       <c r="D56" s="13"/>
       <c r="E56" s="13"/>
       <c r="F56" s="12"/>
       <c r="G56" s="12" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="H56" s="13"/>
       <c r="I56" s="13"/>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B57" s="11" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C57" s="13"/>
       <c r="D57" s="13"/>
@@ -1404,7 +1403,7 @@
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B58" s="11" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C58" s="13"/>
       <c r="D58" s="13"/>
@@ -1416,7 +1415,7 @@
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B59" s="11" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C59" s="13"/>
       <c r="D59" s="13"/>
@@ -1430,7 +1429,7 @@
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B60" s="11" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C60" s="13"/>
       <c r="D60" s="13"/>
@@ -1471,25 +1470,25 @@
         <v>8</v>
       </c>
       <c r="C63" s="6" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D63" s="7" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E63" s="6" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="F63" s="7" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G63" s="6" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="H63" s="7" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="I63" s="6" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1601,20 +1600,20 @@
         <v>31</v>
       </c>
       <c r="E70" s="12" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F70" s="13" t="s">
         <v>31</v>
       </c>
       <c r="G70" s="12" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="H70" s="13"/>
       <c r="I70" s="13"/>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B71" s="11" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C71" s="13"/>
       <c r="D71" s="13"/>
@@ -1626,7 +1625,7 @@
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B72" s="11" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C72" s="13"/>
       <c r="D72" s="13"/>
@@ -1640,7 +1639,7 @@
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B73" s="11" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C73" s="13"/>
       <c r="D73" s="13"/>
@@ -1652,7 +1651,7 @@
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B74" s="11" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C74" s="13"/>
       <c r="D74" s="13"/>
@@ -1664,13 +1663,13 @@
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B75" s="11" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C75" s="13"/>
       <c r="D75" s="13"/>
       <c r="E75" s="13"/>
       <c r="F75" s="12" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G75" s="13"/>
       <c r="H75" s="13"/>
@@ -1678,21 +1677,21 @@
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B76" s="11" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C76" s="13"/>
       <c r="D76" s="13"/>
       <c r="E76" s="13"/>
       <c r="F76" s="12"/>
       <c r="G76" s="12" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="H76" s="13"/>
       <c r="I76" s="13"/>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B77" s="11" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C77" s="13"/>
       <c r="D77" s="13"/>
@@ -1704,7 +1703,7 @@
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B78" s="11" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C78" s="13"/>
       <c r="D78" s="13"/>
@@ -1716,7 +1715,7 @@
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B79" s="11" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C79" s="13"/>
       <c r="D79" s="13"/>
@@ -1730,7 +1729,7 @@
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B80" s="11" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C80" s="13"/>
       <c r="D80" s="13"/>

</xml_diff>

<commit_message>
Add: Hacer tarea Lab Info 2 Martes
</commit_message>
<xml_diff>
--- a/Calendario.xlsx
+++ b/Calendario.xlsx
@@ -511,10 +511,10 @@
   <dimension ref="B2:J80"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J10" activeCellId="0" sqref="J10"/>
+      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="31.43"/>
@@ -1748,7 +1748,7 @@
     <mergeCell ref="E8:E9"/>
     <mergeCell ref="F8:F9"/>
     <mergeCell ref="G8:G9"/>
-    <mergeCell ref="D10:D13"/>
+    <mergeCell ref="D10:D12"/>
     <mergeCell ref="E10:E11"/>
     <mergeCell ref="G10:G11"/>
     <mergeCell ref="F15:F16"/>

</xml_diff>

<commit_message>
No hubo clase de informatica Jueves
</commit_message>
<xml_diff>
--- a/Calendario.xlsx
+++ b/Calendario.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="71">
   <si>
     <t xml:space="preserve">             Dias</t>
   </si>
@@ -513,11 +513,11 @@
   </sheetPr>
   <dimension ref="B2:J80"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J11" activeCellId="0" sqref="J11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F54" activeCellId="0" sqref="F54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="31.43"/>
@@ -1230,8 +1230,8 @@
       <c r="E46" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="F46" s="12" t="s">
-        <v>22</v>
+      <c r="F46" s="13" t="s">
+        <v>31</v>
       </c>
       <c r="G46" s="10" t="s">
         <v>17</v>
@@ -1302,9 +1302,6 @@
       <c r="E50" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="F50" s="13" t="s">
-        <v>31</v>
-      </c>
       <c r="G50" s="12" t="s">
         <v>32</v>
       </c>
@@ -1740,7 +1737,7 @@
       <c r="I80" s="13"/>
     </row>
   </sheetData>
-  <mergeCells count="42">
+  <mergeCells count="41">
     <mergeCell ref="D6:D7"/>
     <mergeCell ref="F6:F7"/>
     <mergeCell ref="D8:D9"/>
@@ -1764,7 +1761,6 @@
     <mergeCell ref="F35:F36"/>
     <mergeCell ref="G36:G38"/>
     <mergeCell ref="D46:D47"/>
-    <mergeCell ref="F46:F47"/>
     <mergeCell ref="D48:D49"/>
     <mergeCell ref="E48:E49"/>
     <mergeCell ref="F48:F49"/>

</xml_diff>